<commit_message>
construct mutil level obj such as balanceTable & finish custom multiObj
</commit_message>
<xml_diff>
--- a/assets/资产负债表.xlsx
+++ b/assets/资产负债表.xlsx
@@ -1,41 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zendu/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDF3A5BD-7418-0A40-993C-1EB09B3D73D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="17780" yWindow="6860" windowWidth="27000" windowHeight="16440" xr2:uid="{E8743597-B463-CE4D-BD51-BA2873CCE887}"/>
+    <workbookView windowWidth="25040" windowHeight="23560"/>
   </bookViews>
   <sheets>
     <sheet name="资产负债表" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>2001年年报</t>
   </si>
@@ -305,130 +284,378 @@
   </si>
   <si>
     <t>负债和股东权益合计(亿元)</t>
-  </si>
-  <si>
-    <t>公告日期</t>
-  </si>
-  <si>
-    <t>2002-04-17</t>
-  </si>
-  <si>
-    <t>2003-03-26</t>
-  </si>
-  <si>
-    <t>2004-03-26</t>
-  </si>
-  <si>
-    <t>2005-04-23</t>
-  </si>
-  <si>
-    <t>2006-04-05</t>
-  </si>
-  <si>
-    <t>2007-04-03</t>
-  </si>
-  <si>
-    <t>2008-03-13</t>
-  </si>
-  <si>
-    <t>2009-03-25</t>
-  </si>
-  <si>
-    <t>2010-04-02</t>
-  </si>
-  <si>
-    <t>2011-03-21</t>
-  </si>
-  <si>
-    <t>2012-04-11</t>
-  </si>
-  <si>
-    <t>2013-03-29</t>
-  </si>
-  <si>
-    <t>2014-03-25</t>
-  </si>
-  <si>
-    <t>2015-04-21</t>
-  </si>
-  <si>
-    <t>2016-03-24</t>
-  </si>
-  <si>
-    <t>2017-04-15</t>
-  </si>
-  <si>
-    <t>2018-03-28</t>
-  </si>
-  <si>
-    <t>2019-03-29</t>
-  </si>
-  <si>
-    <t>2020-04-22</t>
-  </si>
-  <si>
-    <t>2021-03-31</t>
-  </si>
-  <si>
-    <t>数据来源</t>
-  </si>
-  <si>
-    <t>年报报告</t>
-  </si>
-  <si>
-    <t>审计意见(境内)</t>
-  </si>
-  <si>
-    <t>标准无保留意见</t>
-  </si>
-  <si>
-    <t>审计意见(境外)</t>
-  </si>
-  <si>
-    <t>数据来源：东方财富Choice数据</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -436,14 +663,256 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -454,22 +923,63 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 2" xfId="1" xr:uid="{BD6DE954-48A8-8946-8100-86408E982C4E}"/>
+    <cellStyle name="常规 2" xfId="1"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="2" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="3" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="4" builtinId="41"/>
+    <cellStyle name="输入" xfId="5" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="7" builtinId="38"/>
+    <cellStyle name="货币" xfId="8" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="9" builtinId="37"/>
+    <cellStyle name="百分比" xfId="10" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="11" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="12" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="13" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="14" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="15" builtinId="44"/>
+    <cellStyle name="计算" xfId="16" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="17" builtinId="29"/>
+    <cellStyle name="适中" xfId="18" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="19" builtinId="46"/>
+    <cellStyle name="好" xfId="20" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="21" builtinId="30"/>
+    <cellStyle name="汇总" xfId="22" builtinId="25"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="24" builtinId="23"/>
+    <cellStyle name="输出" xfId="25" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="26" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="27" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="28" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="29" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="30" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="31" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="32" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="33" builtinId="9"/>
+    <cellStyle name="标题" xfId="34" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="35" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="36" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="37" builtinId="40"/>
+    <cellStyle name="注释" xfId="38" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="40" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="41" builtinId="51"/>
+    <cellStyle name="超链接" xfId="42" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="43" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="44" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="45" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="46" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="48" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="49" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -518,7 +1028,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -551,26 +1061,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -603,23 +1096,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -761,35 +1237,29 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{075190BA-ACE5-8C43-B7AE-B7B57F98633F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
-    <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
+    <pageSetUpPr fitToPage="1" autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1:U81"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="22" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="22" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="1" customWidth="1"/>
-    <col min="2" max="21" width="16.33203125" style="2" customWidth="1"/>
-    <col min="22" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="29.3333333333333" style="1" customWidth="1"/>
+    <col min="2" max="21" width="16.3333333333333" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="8.83333333333333" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="22" customHeight="1">
+    <row r="1" customHeight="1" spans="2:21">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -851,17 +1321,17 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="22" customHeight="1">
+    <row r="2" customHeight="1" spans="1:1">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="22" customHeight="1">
+    <row r="3" customHeight="1" spans="1:21">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="3">
-        <v>19.559999999999999</v>
+        <v>19.56</v>
       </c>
       <c r="C3" s="3">
         <v>17.8</v>
@@ -915,13 +1385,13 @@
         <v>1120.75</v>
       </c>
       <c r="T3" s="3">
-        <v>132.52000000000001</v>
+        <v>132.52</v>
       </c>
       <c r="U3" s="3">
         <v>360.91</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="22" customHeight="1">
+    <row r="4" customHeight="1" spans="1:21">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -935,12 +1405,12 @@
         <v>1182</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="22" customHeight="1">
+    <row r="5" customHeight="1" spans="1:21">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="C5" s="3">
         <v>0.8</v>
@@ -952,16 +1422,16 @@
         <v>1.47</v>
       </c>
       <c r="F5" s="3">
-        <v>2.0299999999999998</v>
+        <v>2.03</v>
       </c>
       <c r="H5" s="3">
         <v>1.47</v>
       </c>
       <c r="I5" s="3">
-        <v>2.0499999999999998</v>
+        <v>2.05</v>
       </c>
       <c r="J5" s="3">
-        <v>4.0199999999999996</v>
+        <v>4.02</v>
       </c>
       <c r="K5" s="3">
         <v>2.06</v>
@@ -970,7 +1440,7 @@
         <v>2.54</v>
       </c>
       <c r="M5" s="3">
-        <v>2.2200000000000002</v>
+        <v>2.22</v>
       </c>
       <c r="N5" s="3">
         <v>2.97</v>
@@ -997,7 +1467,7 @@
         <v>15.33</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="22" customHeight="1">
+    <row r="6" customHeight="1" spans="1:21">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1011,7 +1481,7 @@
         <v>0.47</v>
       </c>
       <c r="E6" s="3">
-        <v>1.1499999999999999</v>
+        <v>1.15</v>
       </c>
       <c r="F6" s="3">
         <v>1.6</v>
@@ -1029,7 +1499,7 @@
         <v>3.81</v>
       </c>
       <c r="K6" s="3">
-        <v>2.0499999999999998</v>
+        <v>2.05</v>
       </c>
       <c r="L6" s="3">
         <v>2.52</v>
@@ -1062,7 +1532,7 @@
         <v>15.33</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="22" customHeight="1">
+    <row r="7" customHeight="1" spans="1:16">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1112,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="22" customHeight="1">
+    <row r="8" customHeight="1" spans="1:21">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -1135,7 +1605,7 @@
         <v>0.04</v>
       </c>
       <c r="H8" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="I8" s="3">
         <v>7.42</v>
@@ -1150,7 +1620,7 @@
         <v>18.61</v>
       </c>
       <c r="M8" s="3">
-        <v>38.729999999999997</v>
+        <v>38.73</v>
       </c>
       <c r="N8" s="3">
         <v>43.05</v>
@@ -1177,7 +1647,7 @@
         <v>8.98</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="22" customHeight="1">
+    <row r="9" customHeight="1" spans="1:21">
       <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
@@ -1191,7 +1661,7 @@
         <v>1.2</v>
       </c>
       <c r="E9" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="F9" s="3">
         <v>0.51</v>
@@ -1224,7 +1694,7 @@
         <v>1.34</v>
       </c>
       <c r="Q9" s="3">
-        <v>2.1800000000000002</v>
+        <v>2.18</v>
       </c>
       <c r="R9" s="3">
         <v>2.73</v>
@@ -1239,7 +1709,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="22" customHeight="1">
+    <row r="10" customHeight="1" spans="1:19">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -1280,12 +1750,12 @@
         <v>3.44</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="22" customHeight="1">
+    <row r="11" customHeight="1" spans="1:1">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="22" customHeight="1">
+    <row r="12" customHeight="1" spans="1:21">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -1299,13 +1769,13 @@
         <v>1.2</v>
       </c>
       <c r="E12" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="F12" s="3">
         <v>0.51</v>
       </c>
       <c r="G12" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="H12" s="3">
         <v>0.86</v>
@@ -1350,7 +1820,7 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="22" customHeight="1">
+    <row r="13" customHeight="1" spans="1:21">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -1364,7 +1834,7 @@
         <v>12.15</v>
       </c>
       <c r="E13" s="3">
-        <v>16.940000000000001</v>
+        <v>16.94</v>
       </c>
       <c r="F13" s="3">
         <v>18.61</v>
@@ -1415,7 +1885,7 @@
         <v>288.69</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="22" customHeight="1">
+    <row r="14" customHeight="1" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1423,7 +1893,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="22" customHeight="1">
+    <row r="15" customHeight="1" spans="1:21">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1443,7 +1913,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="22" customHeight="1">
+    <row r="16" customHeight="1" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -1454,7 +1924,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="22" customHeight="1">
+    <row r="17" customHeight="1" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -1468,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="22" customHeight="1">
+    <row r="18" customHeight="1" spans="1:21">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -1488,7 +1958,7 @@
         <v>60.2</v>
       </c>
       <c r="G18" s="3">
-        <v>67.510000000000005</v>
+        <v>67.51</v>
       </c>
       <c r="H18" s="3">
         <v>72.72</v>
@@ -1515,7 +1985,7 @@
         <v>475.71</v>
       </c>
       <c r="P18" s="3">
-        <v>650.04999999999995</v>
+        <v>650.05</v>
       </c>
       <c r="Q18" s="3">
         <v>901.81</v>
@@ -1533,12 +2003,12 @@
         <v>1856.52</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="22" customHeight="1">
+    <row r="19" customHeight="1" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="22" customHeight="1">
+    <row r="20" customHeight="1" spans="1:21">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -1567,7 +2037,7 @@
         <v>29.53</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="22" customHeight="1">
+    <row r="21" customHeight="1" spans="1:21">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1575,7 +2045,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="22" customHeight="1">
+    <row r="22" customHeight="1" spans="1:19">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -1583,24 +2053,24 @@
         <v>0.04</v>
       </c>
       <c r="P22" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="Q22" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="R22" s="3">
-        <v>0.28999999999999998</v>
+        <v>0.29</v>
       </c>
       <c r="S22" s="3">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="22" customHeight="1">
+        <v>0.29</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:15">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H23" s="3">
-        <v>0.57999999999999996</v>
+        <v>0.58</v>
       </c>
       <c r="I23" s="3">
         <v>0.42</v>
@@ -1624,7 +2094,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="22" customHeight="1">
+    <row r="24" customHeight="1" spans="1:14">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1665,7 +2135,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="22" customHeight="1">
+    <row r="25" customHeight="1" spans="1:21">
       <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
@@ -1676,12 +2146,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="22" customHeight="1">
+    <row r="26" customHeight="1" spans="1:21">
       <c r="A26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B26" s="3">
-        <v>4.1399999999999997</v>
+        <v>4.14</v>
       </c>
       <c r="C26" s="3">
         <v>4.7</v>
@@ -1714,7 +2184,7 @@
         <v>54.26</v>
       </c>
       <c r="M26" s="3">
-        <v>68.069999999999993</v>
+        <v>68.07</v>
       </c>
       <c r="N26" s="3">
         <v>85.23</v>
@@ -1741,7 +2211,7 @@
         <v>162.25</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="22" customHeight="1">
+    <row r="27" customHeight="1" spans="1:21">
       <c r="A27" s="1" t="s">
         <v>45</v>
       </c>
@@ -1776,13 +2246,13 @@
         <v>2.63</v>
       </c>
       <c r="L27" s="3">
-        <v>2.5099999999999998</v>
+        <v>2.51</v>
       </c>
       <c r="M27" s="3">
         <v>3.93</v>
       </c>
       <c r="N27" s="3">
-        <v>4.5599999999999996</v>
+        <v>4.56</v>
       </c>
       <c r="O27" s="3">
         <v>34.22</v>
@@ -1806,7 +2276,7 @@
         <v>24.47</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="22" customHeight="1">
+    <row r="28" customHeight="1" spans="1:16">
       <c r="A28" s="1" t="s">
         <v>46</v>
       </c>
@@ -1847,7 +2317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="22" customHeight="1">
+    <row r="29" customHeight="1" spans="1:16">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -1858,7 +2328,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="22" customHeight="1">
+    <row r="30" customHeight="1" spans="1:21">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -1875,13 +2345,13 @@
         <v>0.38</v>
       </c>
       <c r="F30" s="3">
-        <v>0.56999999999999995</v>
+        <v>0.57</v>
       </c>
       <c r="G30" s="3">
         <v>0.66</v>
       </c>
       <c r="H30" s="3">
-        <v>2.4900000000000002</v>
+        <v>2.49</v>
       </c>
       <c r="I30" s="3">
         <v>4.45</v>
@@ -1890,16 +2360,16 @@
         <v>4.66</v>
       </c>
       <c r="K30" s="3">
-        <v>4.5199999999999996</v>
+        <v>4.52</v>
       </c>
       <c r="L30" s="3">
         <v>8.08</v>
       </c>
       <c r="M30" s="3">
-        <v>8.6300000000000008</v>
+        <v>8.63</v>
       </c>
       <c r="N30" s="3">
-        <v>35.630000000000003</v>
+        <v>35.63</v>
       </c>
       <c r="O30" s="3">
         <v>35.83</v>
@@ -1911,7 +2381,7 @@
         <v>35.32</v>
       </c>
       <c r="R30" s="3">
-        <v>34.590000000000003</v>
+        <v>34.59</v>
       </c>
       <c r="S30" s="3">
         <v>34.99</v>
@@ -1923,7 +2393,7 @@
         <v>48.17</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="22" customHeight="1">
+    <row r="31" customHeight="1" spans="1:21">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
@@ -1958,7 +2428,7 @@
         <v>0.19</v>
       </c>
       <c r="L31" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="M31" s="3">
         <v>0.1</v>
@@ -1988,7 +2458,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="32" spans="1:21" ht="22" customHeight="1">
+    <row r="32" customHeight="1" spans="1:21">
       <c r="A32" s="1" t="s">
         <v>50</v>
       </c>
@@ -2014,7 +2484,7 @@
         <v>8.25</v>
       </c>
       <c r="O32" s="3">
-        <v>8.2200000000000006</v>
+        <v>8.22</v>
       </c>
       <c r="P32" s="3">
         <v>11.55</v>
@@ -2035,12 +2505,12 @@
         <v>11.23</v>
       </c>
     </row>
-    <row r="33" spans="1:21" ht="22" customHeight="1">
+    <row r="33" customHeight="1" spans="1:1">
       <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="22" customHeight="1">
+    <row r="34" customHeight="1" spans="1:21">
       <c r="A34" s="1" t="s">
         <v>52</v>
       </c>
@@ -2054,7 +2524,7 @@
         <v>12</v>
       </c>
       <c r="E34" s="3">
-        <v>16.010000000000002</v>
+        <v>16.01</v>
       </c>
       <c r="F34" s="3">
         <v>20.38</v>
@@ -2066,7 +2536,7 @@
         <v>32.1</v>
       </c>
       <c r="I34" s="3">
-        <v>35.130000000000003</v>
+        <v>35.13</v>
       </c>
       <c r="J34" s="3">
         <v>41.14</v>
@@ -2075,13 +2545,13 @@
         <v>52.87</v>
       </c>
       <c r="L34" s="3">
-        <v>70.709999999999994</v>
+        <v>70.71</v>
       </c>
       <c r="M34" s="3">
         <v>87.73</v>
       </c>
       <c r="N34" s="3">
-        <v>135.22999999999999</v>
+        <v>135.23</v>
       </c>
       <c r="O34" s="3">
         <v>183.02</v>
@@ -2105,12 +2575,12 @@
         <v>277.44</v>
       </c>
     </row>
-    <row r="35" spans="1:21" ht="22" customHeight="1">
+    <row r="35" customHeight="1" spans="1:21">
       <c r="A35" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B35" s="3">
-        <v>34.630000000000003</v>
+        <v>34.63</v>
       </c>
       <c r="C35" s="3">
         <v>39.31</v>
@@ -2155,7 +2625,7 @@
         <v>863.01</v>
       </c>
       <c r="Q35" s="3">
-        <v>1129.3499999999999</v>
+        <v>1129.35</v>
       </c>
       <c r="R35" s="3">
         <v>1346.1</v>
@@ -2170,12 +2640,12 @@
         <v>2133.96</v>
       </c>
     </row>
-    <row r="36" spans="1:21" ht="22" customHeight="1">
+    <row r="36" customHeight="1" spans="1:1">
       <c r="A36" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:21" ht="22" customHeight="1">
+    <row r="37" customHeight="1" spans="1:15">
       <c r="A37" s="1" t="s">
         <v>55</v>
       </c>
@@ -2183,7 +2653,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="38" spans="1:21" ht="22" customHeight="1">
+    <row r="38" customHeight="1" spans="1:21">
       <c r="A38" s="1" t="s">
         <v>56</v>
       </c>
@@ -2209,10 +2679,10 @@
         <v>110.49</v>
       </c>
       <c r="U38" s="3">
-        <v>142.41999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="22" customHeight="1">
+        <v>142.42</v>
+      </c>
+    </row>
+    <row r="39" customHeight="1" spans="1:21">
       <c r="A39" s="1" t="s">
         <v>57</v>
       </c>
@@ -2241,7 +2711,7 @@
         <v>1.39</v>
       </c>
       <c r="K39" s="3">
-        <v>2.3199999999999998</v>
+        <v>2.32</v>
       </c>
       <c r="L39" s="3">
         <v>1.72</v>
@@ -2274,12 +2744,12 @@
         <v>13.42</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="22" customHeight="1">
+    <row r="40" customHeight="1" spans="1:1">
       <c r="A40" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="22" customHeight="1">
+    <row r="41" customHeight="1" spans="1:21">
       <c r="A41" s="1" t="s">
         <v>59</v>
       </c>
@@ -2311,7 +2781,7 @@
         <v>1.39</v>
       </c>
       <c r="K41" s="3">
-        <v>2.3199999999999998</v>
+        <v>2.32</v>
       </c>
       <c r="L41" s="3">
         <v>1.72</v>
@@ -2344,7 +2814,7 @@
         <v>13.42</v>
       </c>
     </row>
-    <row r="42" spans="1:21" ht="22" customHeight="1">
+    <row r="42" customHeight="1" spans="1:20">
       <c r="A42" s="1" t="s">
         <v>60</v>
       </c>
@@ -2373,7 +2843,7 @@
         <v>29.36</v>
       </c>
       <c r="J42" s="3">
-        <v>35.159999999999997</v>
+        <v>35.16</v>
       </c>
       <c r="K42" s="3">
         <v>47.39</v>
@@ -2400,13 +2870,13 @@
         <v>144.29</v>
       </c>
       <c r="S42" s="3">
-        <v>135.77000000000001</v>
+        <v>135.77</v>
       </c>
       <c r="T42" s="3">
         <v>137.4</v>
       </c>
     </row>
-    <row r="43" spans="1:21" ht="22" customHeight="1">
+    <row r="43" customHeight="1" spans="1:21">
       <c r="A43" s="1" t="s">
         <v>61</v>
       </c>
@@ -2414,7 +2884,7 @@
         <v>133.22</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="22" customHeight="1">
+    <row r="44" customHeight="1" spans="1:21">
       <c r="A44" s="1" t="s">
         <v>62</v>
       </c>
@@ -2425,7 +2895,7 @@
         <v>0.62</v>
       </c>
       <c r="D44" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.56</v>
       </c>
       <c r="E44" s="3">
         <v>0.63</v>
@@ -2437,13 +2907,13 @@
         <v>0.98</v>
       </c>
       <c r="H44" s="3">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="I44" s="3">
         <v>3.61</v>
       </c>
       <c r="J44" s="3">
-        <v>4.6399999999999997</v>
+        <v>4.64</v>
       </c>
       <c r="K44" s="3">
         <v>5</v>
@@ -2470,7 +2940,7 @@
         <v>19.02</v>
       </c>
       <c r="S44" s="3">
-        <v>20.350000000000001</v>
+        <v>20.35</v>
       </c>
       <c r="T44" s="3">
         <v>24.45</v>
@@ -2479,7 +2949,7 @@
         <v>29.81</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="22" customHeight="1">
+    <row r="45" customHeight="1" spans="1:21">
       <c r="A45" s="1" t="s">
         <v>63</v>
       </c>
@@ -2520,7 +2990,7 @@
         <v>24.3</v>
       </c>
       <c r="N45" s="3">
-        <v>33.119999999999997</v>
+        <v>33.12</v>
       </c>
       <c r="O45" s="3">
         <v>21.05</v>
@@ -2532,7 +3002,7 @@
         <v>42.72</v>
       </c>
       <c r="R45" s="3">
-        <v>77.260000000000005</v>
+        <v>77.26</v>
       </c>
       <c r="S45" s="3">
         <v>107.71</v>
@@ -2544,7 +3014,7 @@
         <v>89.2</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="22" customHeight="1">
+    <row r="46" customHeight="1" spans="1:21">
       <c r="A46" s="1" t="s">
         <v>64</v>
       </c>
@@ -2564,7 +3034,7 @@
         <v>3.07</v>
       </c>
       <c r="H46" s="3">
-        <v>4.6500000000000004</v>
+        <v>4.65</v>
       </c>
       <c r="I46" s="3">
         <v>5.76</v>
@@ -2597,7 +3067,7 @@
         <v>30.63</v>
       </c>
       <c r="S46" s="3">
-        <v>34.049999999999997</v>
+        <v>34.05</v>
       </c>
       <c r="T46" s="3">
         <v>35.9</v>
@@ -2606,7 +3076,7 @@
         <v>32.57</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="22" customHeight="1">
+    <row r="47" customHeight="1" spans="1:20">
       <c r="A47" s="1" t="s">
         <v>65</v>
       </c>
@@ -2632,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="22" customHeight="1">
+    <row r="48" customHeight="1" spans="1:20">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -2640,7 +3110,7 @@
         <v>1.65</v>
       </c>
       <c r="C48" s="3">
-        <v>0.56000000000000005</v>
+        <v>0.56</v>
       </c>
       <c r="D48" s="3">
         <v>0.01</v>
@@ -2664,7 +3134,7 @@
         <v>4.47</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="22" customHeight="1">
+    <row r="49" customHeight="1" spans="1:21">
       <c r="A49" s="1" t="s">
         <v>67</v>
       </c>
@@ -2687,7 +3157,7 @@
         <v>3.1</v>
       </c>
       <c r="H49" s="3">
-        <v>4.2300000000000004</v>
+        <v>4.23</v>
       </c>
       <c r="I49" s="3">
         <v>5.76</v>
@@ -2720,7 +3190,7 @@
         <v>30.4</v>
       </c>
       <c r="S49" s="3">
-        <v>33.619999999999997</v>
+        <v>33.62</v>
       </c>
       <c r="T49" s="3">
         <v>31.43</v>
@@ -2729,15 +3199,15 @@
         <v>32.57</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="22" customHeight="1">
+    <row r="50" customHeight="1" spans="1:21">
       <c r="A50" s="1" t="s">
         <v>68</v>
       </c>
       <c r="U50" s="3">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" ht="22" customHeight="1">
+        <v>16.1</v>
+      </c>
+    </row>
+    <row r="51" customHeight="1" spans="1:6">
       <c r="A51" s="1" t="s">
         <v>69</v>
       </c>
@@ -2751,13 +3221,13 @@
         <v>0.05</v>
       </c>
       <c r="E51" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="F51" s="3">
         <v>0.01</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="22" customHeight="1">
+    <row r="52" customHeight="1" spans="1:21">
       <c r="A52" s="1" t="s">
         <v>70</v>
       </c>
@@ -2822,17 +3292,17 @@
         <v>456.74</v>
       </c>
     </row>
-    <row r="53" spans="1:21" ht="22" customHeight="1">
+    <row r="53" customHeight="1" spans="1:1">
       <c r="A53" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="22" customHeight="1">
+    <row r="54" customHeight="1" spans="1:1">
       <c r="A54" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="22" customHeight="1">
+    <row r="55" customHeight="1" spans="1:18">
       <c r="A55" s="1" t="s">
         <v>73</v>
       </c>
@@ -2870,7 +3340,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="56" spans="1:21" ht="22" customHeight="1">
+    <row r="56" customHeight="1" spans="1:21">
       <c r="A56" s="1" t="s">
         <v>74</v>
       </c>
@@ -2881,7 +3351,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="57" spans="1:21" ht="22" customHeight="1">
+    <row r="57" customHeight="1" spans="1:21">
       <c r="A57" s="1" t="s">
         <v>75</v>
       </c>
@@ -2925,7 +3395,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="58" spans="1:21" ht="22" customHeight="1">
+    <row r="58" customHeight="1" spans="1:21">
       <c r="A58" s="1" t="s">
         <v>76</v>
       </c>
@@ -2990,12 +3460,12 @@
         <v>456.75</v>
       </c>
     </row>
-    <row r="59" spans="1:21" ht="22" customHeight="1">
+    <row r="59" customHeight="1" spans="1:1">
       <c r="A59" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:21" ht="22" customHeight="1">
+    <row r="60" customHeight="1" spans="1:21">
       <c r="A60" s="1" t="s">
         <v>78</v>
       </c>
@@ -3060,7 +3530,7 @@
         <v>12.56</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="22" customHeight="1">
+    <row r="61" customHeight="1" spans="1:21">
       <c r="A61" s="1" t="s">
         <v>79</v>
       </c>
@@ -3074,7 +3544,7 @@
         <v>20.14</v>
       </c>
       <c r="E61" s="3">
-        <v>19.239999999999998</v>
+        <v>19.24</v>
       </c>
       <c r="F61" s="3">
         <v>18.46</v>
@@ -3125,7 +3595,7 @@
         <v>13.75</v>
       </c>
     </row>
-    <row r="62" spans="1:21" ht="22" customHeight="1">
+    <row r="62" customHeight="1" spans="1:21">
       <c r="A62" s="1" t="s">
         <v>80</v>
       </c>
@@ -3139,19 +3609,19 @@
         <v>-0.11</v>
       </c>
       <c r="R62" s="3">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.07</v>
       </c>
       <c r="S62" s="3">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.07</v>
       </c>
       <c r="T62" s="3">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.07</v>
       </c>
       <c r="U62" s="3">
         <v>-0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:21" ht="22" customHeight="1">
+    <row r="63" customHeight="1" spans="1:21">
       <c r="A63" s="1" t="s">
         <v>81</v>
       </c>
@@ -3174,7 +3644,7 @@
         <v>12.53</v>
       </c>
       <c r="H63" s="3">
-        <v>8.3800000000000008</v>
+        <v>8.38</v>
       </c>
       <c r="I63" s="3">
         <v>10.01</v>
@@ -3216,7 +3686,7 @@
         <v>201.75</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="22" customHeight="1">
+    <row r="64" customHeight="1" spans="1:21">
       <c r="A64" s="1" t="s">
         <v>82</v>
       </c>
@@ -3227,7 +3697,7 @@
         <v>0.99</v>
       </c>
       <c r="P64" s="3">
-        <v>2.1800000000000002</v>
+        <v>2.18</v>
       </c>
       <c r="Q64" s="3">
         <v>4.21</v>
@@ -3242,10 +3712,10 @@
         <v>8.98</v>
       </c>
       <c r="U64" s="3">
-        <v>9.2799999999999994</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" ht="22" customHeight="1">
+        <v>9.28</v>
+      </c>
+    </row>
+    <row r="65" customHeight="1" spans="1:21">
       <c r="A65" s="1" t="s">
         <v>83</v>
       </c>
@@ -3262,10 +3732,10 @@
         <v>10.07</v>
       </c>
       <c r="F65" s="3">
-        <v>16.649999999999999</v>
+        <v>16.65</v>
       </c>
       <c r="G65" s="3">
-        <v>16.649999999999999</v>
+        <v>16.65</v>
       </c>
       <c r="H65" s="3">
         <v>50.77</v>
@@ -3295,7 +3765,7 @@
         <v>548.79</v>
       </c>
       <c r="Q65" s="3">
-        <v>627.17999999999995</v>
+        <v>627.18</v>
       </c>
       <c r="R65" s="3">
         <v>800.11</v>
@@ -3310,7 +3780,7 @@
         <v>1375.94</v>
       </c>
     </row>
-    <row r="66" spans="1:21" ht="22" customHeight="1">
+    <row r="66" customHeight="1" spans="1:7">
       <c r="A66" s="1" t="s">
         <v>84</v>
       </c>
@@ -3318,7 +3788,7 @@
         <v>6.61</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="22" customHeight="1">
+    <row r="67" customHeight="1" spans="1:6">
       <c r="A67" s="1" t="s">
         <v>85</v>
       </c>
@@ -3332,7 +3802,7 @@
         <v>1.42</v>
       </c>
     </row>
-    <row r="68" spans="1:21" ht="22" customHeight="1">
+    <row r="68" customHeight="1" spans="1:21">
       <c r="A68" s="1" t="s">
         <v>86</v>
       </c>
@@ -3376,7 +3846,7 @@
         <v>426.22</v>
       </c>
       <c r="O68" s="3">
-        <v>534.29999999999995</v>
+        <v>534.3</v>
       </c>
       <c r="P68" s="3">
         <v>639.26</v>
@@ -3388,7 +3858,7 @@
         <v>914.52</v>
       </c>
       <c r="S68" s="3">
-        <v>1128.3900000000001</v>
+        <v>1128.39</v>
       </c>
       <c r="T68" s="3">
         <v>1360.1</v>
@@ -3397,12 +3867,12 @@
         <v>1613.23</v>
       </c>
     </row>
-    <row r="69" spans="1:21" ht="22" customHeight="1">
+    <row r="69" customHeight="1" spans="1:21">
       <c r="A69" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B69" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.07</v>
       </c>
       <c r="C69" s="3">
         <v>0.23</v>
@@ -3441,7 +3911,7 @@
         <v>15.07</v>
       </c>
       <c r="O69" s="3">
-        <v>18.809999999999999</v>
+        <v>18.81</v>
       </c>
       <c r="P69" s="3">
         <v>23.08</v>
@@ -3462,7 +3932,7 @@
         <v>63.98</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="22" customHeight="1">
+    <row r="70" customHeight="1" spans="1:21">
       <c r="A70" s="1" t="s">
         <v>88</v>
       </c>
@@ -3491,7 +3961,7 @@
         <v>115.03</v>
       </c>
       <c r="J70" s="3">
-        <v>146.52000000000001</v>
+        <v>146.52</v>
       </c>
       <c r="K70" s="3">
         <v>185.49</v>
@@ -3527,12 +3997,12 @@
         <v>1677.21</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="22" customHeight="1">
+    <row r="71" customHeight="1" spans="1:21">
       <c r="A71" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B71" s="3">
-        <v>34.630000000000003</v>
+        <v>34.63</v>
       </c>
       <c r="C71" s="3">
         <v>39.31</v>
@@ -3577,7 +4047,7 @@
         <v>863.01</v>
       </c>
       <c r="Q71" s="3">
-        <v>1129.3499999999999</v>
+        <v>1129.35</v>
       </c>
       <c r="R71" s="3">
         <v>1346.1</v>
@@ -3592,215 +4062,9 @@
         <v>2133.96</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="22" customHeight="1">
-      <c r="A72" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="J72" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="K72" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L72" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="M72" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="N72" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="O72" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="P72" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q72" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="R72" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="S72" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="T72" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="U72" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" ht="22" customHeight="1">
-      <c r="A73" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="J73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="K73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="L73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="M73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="N73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="O73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="P73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="R73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="S73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="T73" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="U73" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" ht="22" customHeight="1">
-      <c r="A74" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="K74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="L74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="M74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="O74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="P74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="R74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="S74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="T74" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="U74" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" ht="22" customHeight="1">
-      <c r="A75" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" ht="22" customHeight="1">
-      <c r="A81" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="1" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>